<commit_message>
modified Table 2 and 3
outcomes available
</commit_message>
<xml_diff>
--- a/i_test/test_D4_analytical_dataset/D3_study_population.xlsx
+++ b/i_test/test_D4_analytical_dataset/D3_study_population.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>person_id</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>gender</t>
+  </si>
+  <si>
+    <t>number_previous_bleedings</t>
   </si>
 </sst>
 </file>
@@ -378,15 +381,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,8 +417,11 @@
       <c r="I1" t="s">
         <v>12</v>
       </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -437,8 +443,11 @@
       <c r="G2">
         <v>120</v>
       </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -457,8 +466,11 @@
       <c r="G3">
         <v>230</v>
       </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -476,6 +488,9 @@
       </c>
       <c r="G4">
         <v>220</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>